<commit_message>
Added more details on Ricardo Palmer example
</commit_message>
<xml_diff>
--- a/examples/palma.xlsx
+++ b/examples/palma.xlsx
@@ -21,6 +21,112 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
   <si>
+    <t>en</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[YOU  NEED  TO  DELETE  THE  SPACE  AFTER “media/”  IN “org/media/ lists” .  OTHERWISE  THE LINK DOES NOT WORK.  THAT SPACE  IS  NOT  IN  THE  ORIGINAL  VERSION  OF  MY  MANUSCRIPT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kim, K.C., Pratt, H.D. &amp; Stojanovich, C.J. (1986) The sucking lice of North America—An illustrated manual for identification. The Pennsylvania State University Press, University Park and London. xii + 241 pp. </t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1017/ S0031182000058078</t>
+  </si>
+  <si>
+    <t>[WRONG  DOI..!]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nelson, B.C. &amp; Murray, M.D. (1971) The distribution of Mallophaga on the domestic pigeon (Columba livia). International Journal for Parasitology, 1, 21–29, 2 pls. </t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/0020-7519(71)90042-7</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/S1055-7903(03)00227-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Causton, C.E., Peck, S.B., Sinclair, B.J., Roque-Albelo, L., Hodgson, C.J. &amp; Landry, B. (2006) Alien insects: threats and implications for conservation of Galápagos Islands. Annals of the Entomological Society of America, 99, 121–143. </t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1603/0013-8746(2006)099[0121:aitaif]2.0.co;2</t>
+  </si>
+  <si>
+    <t>[NOT found]</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.3989/graellsia.1996.v52.i0.373</t>
+  </si>
+  <si>
+    <t>[WRONG  PAPER  and JOURNAL..!]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clay, T. (1949) Systematic notes on the Piaget collections of Mallophaga.—Part I. Annals and magazine of natural history (Series 12), 2, 811–838, 895–921. </t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1080/00222934908654034</t>
+  </si>
+  <si>
+    <t>[This DOI refers to Part II]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clay, T. (1966) A new species of Strigiphilus (Philopteridae: Mallophaga). Pacific Insects, 8(4), 835–847. </t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/ 10.1111/j.1440-6055.1966.tb00671.x</t>
+  </si>
+  <si>
+    <t>[WRONG  PAPER  and  JOURNAL..!]</t>
+  </si>
+  <si>
+    <t>Harrison, L. (1916) The genera and species of Mallophaga. Parasitology, 9(1), 1–156. http://dx.doi.org/10.1017/ S0031182000005989   [NOT found]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hellmayr, C.E. &amp; Conover, B. (1948) Catalogue of birds of the Americas and the adjacent islands. Zoological Series, Field Museum of Natural History, 13(1) No 2, 1–434. </t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.2307/4080645</t>
+  </si>
+  <si>
+    <t>[WRONG  BOOK..!]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palma, R.L. &amp; Price, R.D. (2006) Lice of the genus Philopterus Nitzsch (Phthiraptera: Ischnocera: Philopteridae) parasitic on hosts of the genus Emberiza (Passeriformes: Emberizidae). New Zealand Journal of Zoology, 33, 1–6. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perry, R. (Ed.) (1984) Key environments—Galapagos. International Union for Conservation of Nature and Natural Resources &amp; Pergamon Press, Oxford. x + 321 pp. </t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1017/S0041977X00039276</t>
+  </si>
+  <si>
+    <t>[WRONG  Key environments..!!]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pilgrim, R.L.C. (1976) Mallophaga on the rock pigeon (Columba livia) in New Zealand, with a key to their identification. New Zealand Entomologist, 6(2), 160–164. </t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1111/j.1755-0998.2008.02473.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santiago-Alarcón, D., Whiteman, N.K., Parker, P.G., Ricklefs, R.E. &amp; Valkiūnas, G. (2008) Patterns of parasite abundance and distribution in island populations of Galapagos endemic birds. Journal of Parasitology, 94(3), 584–590. </t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/ 10.1645/GE-1351.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thompson, G.B. (1937b) Further notes on the association of Hippoboscidae and Mallophaga.—II. Mallophaga associated with insects other than Hippoboscidae. Annals and magazine of natural history (Series 10), 20, 441–444. </t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/ 10.1080/00222933708655366</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1007/BF00261221</t>
+  </si>
+  <si>
+    <t>Heraty, J.M. &amp; Herrera, H.W. (2011) CDF Checklist of Galápagos ants, bees, wasps and related groups—FCD Lista de especies de hormigas, abejas, avispas y otros grupos relacionados de Galápagos. Pp. 1–8. In: Bungartz, F., Herrera, H., Jaramillo, P., Tirado, N., Jiménez-Uzcátegui, G., Ruiz, D., Guézou, A. &amp; Ziemmeck, F. (Eds.), Charles Darwin Foundation Galapagos species checklist—Lista de especies de Galápagos de la Fundación Charles Darwin. Charles Darwin Foundation / Fundación Charles Darwin, Puerto Ayora, Galápagos Islands. Available from: http://checklists.datazone.darwinfoundation.org/media/ lists/download/2011_Heraty_et_al_Galapagos_Hymenoptera_Checklist.pdf</t>
+  </si>
+  <si>
     <t>DOI now OK (article has just gone online)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -48,10 +154,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Citation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>DOI</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -106,108 +208,6 @@
   </si>
   <si>
     <t>http://dx.doi.org/ 10.1080/03014223.1994.9517471</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palma, R.L. &amp; Price, R.D. (2006) Lice of the genus Philopterus Nitzsch (Phthiraptera: Ischnocera: Philopteridae) parasitic on hosts of the genus Emberiza (Passeriformes: Emberizidae). New Zealand Journal of Zoology, 33, 1–6. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perry, R. (Ed.) (1984) Key environments—Galapagos. International Union for Conservation of Nature and Natural Resources &amp; Pergamon Press, Oxford. x + 321 pp. </t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1017/S0041977X00039276</t>
-  </si>
-  <si>
-    <t>[WRONG  Key environments..!!]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pilgrim, R.L.C. (1976) Mallophaga on the rock pigeon (Columba livia) in New Zealand, with a key to their identification. New Zealand Entomologist, 6(2), 160–164. </t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1111/j.1755-0998.2008.02473.x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Santiago-Alarcón, D., Whiteman, N.K., Parker, P.G., Ricklefs, R.E. &amp; Valkiūnas, G. (2008) Patterns of parasite abundance and distribution in island populations of Galapagos endemic birds. Journal of Parasitology, 94(3), 584–590. </t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/ 10.1645/GE-1351.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thompson, G.B. (1937b) Further notes on the association of Hippoboscidae and Mallophaga.—II. Mallophaga associated with insects other than Hippoboscidae. Annals and magazine of natural history (Series 10), 20, 441–444. </t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/ 10.1080/00222933708655366</t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1007/BF00261221</t>
-  </si>
-  <si>
-    <t>Heraty, J.M. &amp; Herrera, H.W. (2011) CDF Checklist of Galápagos ants, bees, wasps and related groups—FCD Lista de especies de hormigas, abejas, avispas y otros grupos relacionados de Galápagos. Pp. 1–8. In: Bungartz, F., Herrera, H., Jaramillo, P., Tirado, N., Jiménez-Uzcátegui, G., Ruiz, D., Guézou, A. &amp; Ziemmeck, F. (Eds.), Charles Darwin Foundation Galapagos species checklist—Lista de especies de Galápagos de la Fundación Charles Darwin. Charles Darwin Foundation / Fundación Charles Darwin, Puerto Ayora, Galápagos Islands. Available from: http://checklists.datazone.darwinfoundation.org/media/ lists/download/2011_Heraty_et_al_Galapagos_Hymenoptera_Checklist.pdf</t>
-  </si>
-  <si>
-    <t>[YOU  NEED  TO  DELETE  THE  SPACE  AFTER “media/”  IN “org/media/ lists” .  OTHERWISE  THE LINK DOES NOT WORK.  THAT SPACE  IS  NOT  IN  THE  ORIGINAL  VERSION  OF  MY  MANUSCRIPT]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kim, K.C., Pratt, H.D. &amp; Stojanovich, C.J. (1986) The sucking lice of North America—An illustrated manual for identification. The Pennsylvania State University Press, University Park and London. xii + 241 pp. </t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1017/ S0031182000058078</t>
-  </si>
-  <si>
-    <t>[WRONG  DOI..!]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nelson, B.C. &amp; Murray, M.D. (1971) The distribution of Mallophaga on the domestic pigeon (Columba livia). International Journal for Parasitology, 1, 21–29, 2 pls. </t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1016/0020-7519(71)90042-7</t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1016/S1055-7903(03)00227-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Causton, C.E., Peck, S.B., Sinclair, B.J., Roque-Albelo, L., Hodgson, C.J. &amp; Landry, B. (2006) Alien insects: threats and implications for conservation of Galápagos Islands. Annals of the Entomological Society of America, 99, 121–143. </t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1603/0013-8746(2006)099[0121:aitaif]2.0.co;2</t>
-  </si>
-  <si>
-    <t>[NOT found]</t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.3989/graellsia.1996.v52.i0.373</t>
-  </si>
-  <si>
-    <t>[WRONG  PAPER  and JOURNAL..!]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clay, T. (1949) Systematic notes on the Piaget collections of Mallophaga.—Part I. Annals and magazine of natural history (Series 12), 2, 811–838, 895–921. </t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1080/00222934908654034</t>
-  </si>
-  <si>
-    <t>[This DOI refers to Part II]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clay, T. (1966) A new species of Strigiphilus (Philopteridae: Mallophaga). Pacific Insects, 8(4), 835–847. </t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/ 10.1111/j.1440-6055.1966.tb00671.x</t>
-  </si>
-  <si>
-    <t>[WRONG  PAPER  and  JOURNAL..!]</t>
-  </si>
-  <si>
-    <t>Harrison, L. (1916) The genera and species of Mallophaga. Parasitology, 9(1), 1–156. http://dx.doi.org/10.1017/ S0031182000005989   [NOT found]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hellmayr, C.E. &amp; Conover, B. (1948) Catalogue of birds of the Americas and the adjacent islands. Zoological Series, Field Museum of Natural History, 13(1) No 2, 1–434. </t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.2307/4080645</t>
-  </si>
-  <si>
-    <t>[WRONG  BOOK..!]</t>
   </si>
 </sst>
 </file>
@@ -607,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -622,94 +622,94 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="52">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="65">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="39">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="26">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="39">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="156">
@@ -717,77 +717,77 @@
         <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="65">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52">
@@ -795,13 +795,13 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39">
@@ -815,7 +815,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39">
@@ -826,10 +826,10 @@
         <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52">
@@ -840,10 +840,10 @@
         <v>30</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52">
@@ -854,45 +854,40 @@
         <v>32</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="65">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52">
       <c r="A20" s="2" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="39"/>
-    <row r="25" spans="1:4" ht="26"/>
-    <row r="26" spans="1:4" ht="39"/>
-    <row r="30" spans="1:4" ht="26"/>
-    <row r="31" spans="1:4" ht="39"/>
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>